<commit_message>
create Naver Movie ER-Diagram, Table
</commit_message>
<xml_diff>
--- a/Movie.xlsx
+++ b/Movie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Devs\DataBasePractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A3EFB9-87A5-4EE2-A160-B85B9E126DBF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E84B18-B5BF-4191-BBF7-BE60FB187628}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180" tabRatio="859" xr2:uid="{CEC57BE9-2B5B-418C-824D-F4DB02118143}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180" tabRatio="859" firstSheet="20" activeTab="20" xr2:uid="{CEC57BE9-2B5B-418C-824D-F4DB02118143}"/>
   </bookViews>
   <sheets>
     <sheet name="각 테이블 정보" sheetId="19" r:id="rId1"/>
@@ -33,7 +33,7 @@
     <sheet name="영화_제작사" sheetId="15" state="hidden" r:id="rId18"/>
     <sheet name="배급사" sheetId="12" state="hidden" r:id="rId19"/>
     <sheet name="배급" sheetId="13" state="hidden" r:id="rId20"/>
-    <sheet name="포토" sheetId="30" r:id="rId21"/>
+    <sheet name="사진" sheetId="30" r:id="rId21"/>
     <sheet name="포토_스틸컷" sheetId="16" state="hidden" r:id="rId22"/>
     <sheet name="포토_프로모션" sheetId="17" state="hidden" r:id="rId23"/>
     <sheet name="포토_포스터" sheetId="18" state="hidden" r:id="rId24"/>
@@ -44,7 +44,7 @@
     <sheet name="동영상_인터뷰" sheetId="22" state="hidden" r:id="rId29"/>
     <sheet name="명대사" sheetId="24" r:id="rId30"/>
     <sheet name="공통코드" sheetId="27" r:id="rId31"/>
-    <sheet name="포토_댓글" sheetId="37" r:id="rId32"/>
+    <sheet name="사진_댓글" sheetId="37" r:id="rId32"/>
     <sheet name="동영상_댓글" sheetId="38" r:id="rId33"/>
     <sheet name="평점" sheetId="39" r:id="rId34"/>
   </sheets>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="420">
   <si>
     <t>감독</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -866,10 +866,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>등록일</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>등록자명</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1175,10 +1171,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>포토 종류</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>회사ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1468,10 +1460,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>평점작성일</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>MR-20230306-00001</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1534,6 +1522,30 @@
   </si>
   <si>
     <t>PD-20230306-00012</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>종류</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록시간</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>평점작성시간</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>006_01</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>006_02</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>006_03</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1743,6 +1755,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1751,12 +1769,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2075,7 +2087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D0C44D-1C6F-4701-B848-A043E37398C4}">
   <dimension ref="D3:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
@@ -2083,12 +2095,12 @@
   <sheetData>
     <row r="3" spans="4:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="4:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="15"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="17"/>
       <c r="J4" s="3"/>
     </row>
     <row r="5" spans="4:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2137,13 +2149,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>93</v>
@@ -2154,7 +2166,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>32</v>
@@ -2163,7 +2175,7 @@
         <v>90</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E2" t="s">
         <v>51</v>
@@ -2171,7 +2183,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>32</v>
@@ -2180,7 +2192,7 @@
         <v>91</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E3" t="s">
         <v>51</v>
@@ -2188,16 +2200,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E4" t="s">
         <v>51</v>
@@ -2205,16 +2217,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E5" t="s">
         <v>51</v>
@@ -2222,16 +2234,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E6" t="s">
         <v>51</v>
@@ -2239,16 +2251,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E7" t="s">
         <v>76</v>
@@ -2256,16 +2268,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E8" t="s">
         <v>77</v>
@@ -2273,16 +2285,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E9" t="s">
         <v>78</v>
@@ -2290,16 +2302,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E10" t="s">
         <v>51</v>
@@ -2307,16 +2319,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E11" t="s">
         <v>51</v>
@@ -2324,16 +2336,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E12" t="s">
         <v>51</v>
@@ -2341,16 +2353,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E13" t="s">
         <v>51</v>
@@ -2675,15 +2687,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B2" t="s">
         <v>102</v>
@@ -2691,7 +2703,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B3" t="s">
         <v>101</v>
@@ -2699,7 +2711,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B4" t="s">
         <v>109</v>
@@ -2707,7 +2719,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B5" t="s">
         <v>110</v>
@@ -2715,7 +2727,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B6" t="s">
         <v>114</v>
@@ -2723,7 +2735,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B7" t="s">
         <v>115</v>
@@ -2731,7 +2743,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B8" t="s">
         <v>120</v>
@@ -2739,7 +2751,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B9" t="s">
         <v>121</v>
@@ -2768,128 +2780,128 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="G9" s="2"/>
     </row>
@@ -2911,7 +2923,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -3209,7 +3221,7 @@
   <dimension ref="A1:AB60"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:I1"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3262,7 +3274,7 @@
         <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E2">
         <v>116</v>
@@ -3271,7 +3283,7 @@
         <v>14</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H2" t="s">
         <v>16</v>
@@ -3291,7 +3303,7 @@
         <v>19</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E3">
         <v>113</v>
@@ -3300,7 +3312,7 @@
         <v>14</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H3" t="s">
         <v>22</v>
@@ -3320,7 +3332,7 @@
         <v>25</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E4">
         <v>100</v>
@@ -3329,7 +3341,7 @@
         <v>27</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H4" t="s">
         <v>29</v>
@@ -3455,8 +3467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E40352F-6520-4D2F-A475-9DC9D4E0A678}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3476,7 +3488,7 @@
         <v>31</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>313</v>
+        <v>414</v>
       </c>
       <c r="D1" t="s">
         <v>126</v>
@@ -3487,13 +3499,13 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D2" t="s">
         <v>129</v>
@@ -3504,13 +3516,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D3" t="s">
         <v>135</v>
@@ -3521,13 +3533,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D4" t="s">
         <v>136</v>
@@ -3539,13 +3551,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D5" t="s">
         <v>137</v>
@@ -3557,13 +3569,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D6" t="s">
         <v>138</v>
@@ -3575,13 +3587,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D7" t="s">
         <v>129</v>
@@ -3592,13 +3604,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D8" t="s">
         <v>135</v>
@@ -3609,13 +3621,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D9" t="s">
         <v>136</v>
@@ -3626,13 +3638,13 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D10" t="s">
         <v>137</v>
@@ -3643,13 +3655,13 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D11" t="s">
         <v>138</v>
@@ -3660,13 +3672,13 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D12" t="s">
         <v>129</v>
@@ -3677,13 +3689,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D13" t="s">
         <v>135</v>
@@ -3694,13 +3706,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D14" t="s">
         <v>136</v>
@@ -3711,13 +3723,13 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D15" t="s">
         <v>137</v>
@@ -3728,13 +3740,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D16" t="s">
         <v>138</v>
@@ -3745,13 +3757,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D17" t="s">
         <v>129</v>
@@ -3762,13 +3774,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D18" t="s">
         <v>135</v>
@@ -3779,13 +3791,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D19" t="s">
         <v>136</v>
@@ -3796,13 +3808,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D20" t="s">
         <v>137</v>
@@ -3813,13 +3825,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D21" t="s">
         <v>138</v>
@@ -3830,13 +3842,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D22" t="s">
         <v>129</v>
@@ -3847,13 +3859,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D23" t="s">
         <v>135</v>
@@ -3864,13 +3876,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D24" t="s">
         <v>136</v>
@@ -3881,13 +3893,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D25" t="s">
         <v>137</v>
@@ -3898,13 +3910,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D26" t="s">
         <v>138</v>
@@ -3915,13 +3927,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D27" t="s">
         <v>129</v>
@@ -3932,13 +3944,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D28" t="s">
         <v>135</v>
@@ -3949,13 +3961,13 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D29" t="s">
         <v>136</v>
@@ -3966,13 +3978,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D30" t="s">
         <v>137</v>
@@ -3983,13 +3995,13 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D31" t="s">
         <v>138</v>
@@ -4000,13 +4012,13 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D32" t="s">
         <v>129</v>
@@ -4017,13 +4029,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D33" t="s">
         <v>135</v>
@@ -4034,13 +4046,13 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D34" t="s">
         <v>136</v>
@@ -4051,13 +4063,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D35" t="s">
         <v>137</v>
@@ -4068,13 +4080,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D36" t="s">
         <v>138</v>
@@ -4691,8 +4703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CD6C4A1-00B1-457A-82A7-9FC204325BD9}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4714,7 +4726,7 @@
         <v>31</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D1" t="s">
         <v>180</v>
@@ -4740,7 +4752,7 @@
         <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D2" t="s">
         <v>188</v>
@@ -4766,7 +4778,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D3" t="s">
         <v>189</v>
@@ -4792,7 +4804,7 @@
         <v>32</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D4" t="s">
         <v>190</v>
@@ -4818,7 +4830,7 @@
         <v>32</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D5" t="s">
         <v>191</v>
@@ -4844,7 +4856,7 @@
         <v>33</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D6" t="s">
         <v>204</v>
@@ -4870,7 +4882,7 @@
         <v>33</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D7" t="s">
         <v>205</v>
@@ -4896,7 +4908,7 @@
         <v>34</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D8" t="s">
         <v>214</v>
@@ -4922,7 +4934,7 @@
         <v>34</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D9" t="s">
         <v>213</v>
@@ -4948,7 +4960,7 @@
         <v>34</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D10" t="s">
         <v>189</v>
@@ -4974,7 +4986,7 @@
         <v>32</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D11" t="s">
         <v>200</v>
@@ -5000,7 +5012,7 @@
         <v>32</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D12" t="s">
         <v>201</v>
@@ -5026,7 +5038,7 @@
         <v>33</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D13" t="s">
         <v>210</v>
@@ -5052,7 +5064,7 @@
         <v>33</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D14" t="s">
         <v>211</v>
@@ -5332,7 +5344,7 @@
       <c r="B16" s="5"/>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C17" s="16"/>
+      <c r="C17" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -5569,10 +5581,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="B1" t="s">
         <v>238</v>
-      </c>
-      <c r="B1" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -5580,7 +5592,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -5588,7 +5600,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -5596,7 +5608,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -5609,8 +5621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C556EBE5-CE6B-48DD-9C44-50EF44BF6D9A}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5632,7 +5644,7 @@
         <v>31</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -5641,36 +5653,36 @@
         <v>222</v>
       </c>
       <c r="F1" t="s">
+        <v>415</v>
+      </c>
+      <c r="G1" t="s">
         <v>223</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>224</v>
-      </c>
-      <c r="H1" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D2" s="17" t="s">
+        <v>410</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="E2" t="s">
         <v>230</v>
-      </c>
-      <c r="E2" t="s">
-        <v>231</v>
       </c>
       <c r="F2" t="s">
         <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H2">
         <v>61</v>
@@ -5678,25 +5690,25 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="D3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H3">
         <v>36</v>
@@ -5704,25 +5716,25 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D4" t="s">
+        <v>234</v>
+      </c>
+      <c r="E4" t="s">
+        <v>230</v>
+      </c>
+      <c r="F4" t="s">
         <v>235</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>231</v>
-      </c>
-      <c r="F4" t="s">
-        <v>236</v>
-      </c>
-      <c r="G4" t="s">
-        <v>232</v>
       </c>
       <c r="H4">
         <v>5</v>
@@ -5730,25 +5742,25 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="D5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E5" t="s">
+        <v>230</v>
+      </c>
+      <c r="F5" t="s">
+        <v>235</v>
+      </c>
+      <c r="G5" t="s">
         <v>231</v>
-      </c>
-      <c r="F5" t="s">
-        <v>236</v>
-      </c>
-      <c r="G5" t="s">
-        <v>232</v>
       </c>
       <c r="H5">
         <v>5</v>
@@ -5768,7 +5780,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5780,18 +5792,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B1" t="s">
         <v>244</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>245</v>
-      </c>
-      <c r="C1" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -5802,32 +5814,32 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B4" t="s">
         <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B5" t="s">
         <v>250</v>
-      </c>
-      <c r="B5" t="s">
-        <v>251</v>
       </c>
       <c r="C5" t="s">
         <v>51</v>
@@ -5835,65 +5847,65 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B7" t="s">
         <v>253</v>
       </c>
-      <c r="B7" t="s">
-        <v>254</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B11" t="s">
         <v>295</v>
-      </c>
-      <c r="B11" t="s">
-        <v>296</v>
       </c>
       <c r="C11" t="s">
         <v>51</v>
@@ -5901,43 +5913,43 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B12" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B13" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B14" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="B15" t="s">
         <v>302</v>
-      </c>
-      <c r="B15" t="s">
-        <v>303</v>
       </c>
       <c r="C15" t="s">
         <v>51</v>
@@ -5945,54 +5957,54 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B16" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B18" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B19" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B20" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C20" t="s">
         <v>51</v>
@@ -6000,65 +6012,65 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B21" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B22" t="s">
         <v>94</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B23" t="s">
         <v>95</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B24" t="s">
         <v>63</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B25" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B26" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C26" t="s">
         <v>51</v>
@@ -6066,35 +6078,35 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>376</v>
+        <v>417</v>
       </c>
       <c r="B27" t="s">
+        <v>371</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>373</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>377</v>
+        <v>418</v>
       </c>
       <c r="B28" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>378</v>
+        <v>419</v>
       </c>
       <c r="B29" t="s">
         <v>95</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
   </sheetData>
@@ -6122,28 +6134,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>125</v>
       </c>
       <c r="C1" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1" t="s">
+        <v>381</v>
+      </c>
+      <c r="E1" t="s">
         <v>382</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>383</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>384</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>385</v>
-      </c>
-      <c r="G1" t="s">
-        <v>386</v>
-      </c>
-      <c r="H1" t="s">
-        <v>387</v>
       </c>
     </row>
   </sheetData>
@@ -6156,8 +6168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87E7CB49-9925-47AD-A1B9-C78A62E95EFE}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6173,45 +6185,45 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>179</v>
       </c>
       <c r="C1" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1" t="s">
+        <v>381</v>
+      </c>
+      <c r="E1" t="s">
         <v>382</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>383</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>384</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>385</v>
-      </c>
-      <c r="G1" t="s">
-        <v>386</v>
-      </c>
-      <c r="H1" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B2" t="s">
         <v>186</v>
       </c>
       <c r="C2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E2" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -6225,19 +6237,19 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B3" t="s">
         <v>186</v>
       </c>
       <c r="C3" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D3" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="E3" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -6260,7 +6272,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6274,7 +6286,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>31</v>
@@ -6283,24 +6295,24 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F1" t="s">
-        <v>399</v>
+        <v>416</v>
       </c>
       <c r="G1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="H1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -6309,13 +6321,13 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="E2" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="F2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="G2">
         <v>615</v>
@@ -6326,7 +6338,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
@@ -6335,13 +6347,13 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="E3" t="s">
+        <v>406</v>
+      </c>
+      <c r="F3" t="s">
         <v>409</v>
-      </c>
-      <c r="F3" t="s">
-        <v>412</v>
       </c>
       <c r="G3">
         <v>391</v>
@@ -6352,7 +6364,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="B4" t="s">
         <v>33</v>
@@ -6361,10 +6373,10 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="E4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="F4" t="s">
         <v>14</v>
@@ -6378,7 +6390,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="B5" t="s">
         <v>33</v>
@@ -6387,10 +6399,10 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="E5" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="F5" t="s">
         <v>14</v>
@@ -6413,7 +6425,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6423,7 +6435,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>31</v>
@@ -6455,7 +6467,7 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -6701,7 +6713,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B1" t="s">
         <v>41</v>
@@ -6743,7 +6755,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B4" t="s">
         <v>43</v>
@@ -6757,7 +6769,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B5" t="s">
         <v>45</v>
@@ -6771,7 +6783,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B6" t="s">
         <v>46</v>
@@ -6785,10 +6797,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B7" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C7" t="s">
         <v>59</v>
@@ -6799,10 +6811,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B8" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C8" t="s">
         <v>60</v>
@@ -6813,10 +6825,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B9" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C9" t="s">
         <v>73</v>
@@ -6827,10 +6839,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B10" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C10" t="s">
         <v>74</v>
@@ -6841,10 +6853,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B11" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C11" t="s">
         <v>75</v>
@@ -6855,10 +6867,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B12" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C12" t="s">
         <v>83</v>
@@ -6869,10 +6881,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B13" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C13" t="s">
         <v>84</v>

</xml_diff>